<commit_message>
Classwork as of 9/23
</commit_message>
<xml_diff>
--- a/Copy of HomeSales.xlsx
+++ b/Copy of HomeSales.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e5b61916b0c219c5/Desktop/QMBE_1320_Laura_Hardy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e5b61916b0c219c5/Desktop/QMBE_1320_Laura_Hardy/QMBE1320_Laura_Hardy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{4D2724FF-6352-4070-87DA-13A39D434B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87F3E20A-6BAB-4959-A08B-F699C5B92632}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{4D2724FF-6352-4070-87DA-13A39D434B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6192C87-C60C-4035-8F42-477C482BB7D7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,7 +156,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -168,9 +168,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -187,6 +185,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -479,7 +481,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,7 +490,7 @@
     <col min="2" max="2" width="16.109375" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -500,7 +502,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="5"/>
+      <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -514,7 +516,7 @@
       <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <f>AVERAGE(B2:B13)</f>
         <v>219937.5</v>
       </c>
@@ -532,7 +534,7 @@
       <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <f>MEDIAN(B2:B13)</f>
         <v>203750</v>
       </c>
@@ -550,7 +552,7 @@
       <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="6" cm="1">
+      <c r="E4" s="5" cm="1">
         <f t="array" ref="E4:E5">_xlfn.MODE.MULT(B2:B13)</f>
         <v>138000</v>
       </c>
@@ -566,7 +568,7 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>254000</v>
       </c>
       <c r="F5" s="2"/>
@@ -583,7 +585,7 @@
       <c r="D6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="2">
         <f>MAX(B2:B13)-MIN(B2:B13)</f>
         <v>348250</v>
       </c>
@@ -601,7 +603,7 @@
       <c r="D7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="2">
         <f>_xlfn.VAR.S(B2:B13)</f>
         <v>9037501420.454546</v>
       </c>
@@ -623,7 +625,7 @@
       <c r="D8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="2">
         <f>_xlfn.STDEV.S(B2:B13)</f>
         <v>95065.774180062013</v>
       </c>
@@ -639,7 +641,7 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
+      <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="K9" s="3"/>
     </row>
@@ -654,7 +656,7 @@
       <c r="D10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="2">
         <f>(E8/E2)*100</f>
         <v>43.223995080448766</v>
       </c>
@@ -670,7 +672,7 @@
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="5"/>
+      <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="K11" s="3"/>
     </row>
@@ -685,7 +687,7 @@
       <c r="D12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="2">
         <f>_xlfn.PERCENTILE.EXC(B2:B13,0.85)</f>
         <v>305912.49999999983</v>
       </c>
@@ -701,7 +703,7 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="K13" s="3"/>
     </row>
@@ -712,7 +714,10 @@
       <c r="D14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="E14" s="2">
+        <f>_xlfn.QUARTILE.EXC(B2:B13,1)</f>
+        <v>139000</v>
+      </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -722,17 +727,28 @@
       <c r="D15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="5"/>
+      <c r="E15" s="2">
+        <f>_xlfn.PERCENTILE.INC(B2:B13,0.5)</f>
+        <v>203750</v>
+      </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D16" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="4:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <f>_xlfn.QUARTILE.EXC(B2:B13,3)</f>
+        <v>256625</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D17" s="4" t="s">
         <v>13</v>
+      </c>
+      <c r="E17">
+        <f>E16-E14</f>
+        <v>117625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>